<commit_message>
add create order function part 3
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -81,7 +81,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -93,7 +93,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -468,8 +467,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="40.7109375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
   <cols>
-    <col width="40.7109375" customWidth="1" style="1" min="1" max="5"/>
-    <col width="40.7109375" customWidth="1" style="1" min="6" max="16384"/>
+    <col width="40.7109375" customWidth="1" style="1" min="1" max="6"/>
+    <col width="40.7109375" customWidth="1" style="1" min="7" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customFormat="1" customHeight="1" s="2">
@@ -494,7 +493,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="5">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>ва</t>
@@ -536,8 +535,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="40.7109375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
   <cols>
-    <col width="40.7109375" customWidth="1" style="1" min="1" max="5"/>
-    <col width="40.7109375" customWidth="1" style="1" min="6" max="16384"/>
+    <col width="40.7109375" customWidth="1" style="1" min="1" max="6"/>
+    <col width="40.7109375" customWidth="1" style="1" min="7" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customFormat="1" customHeight="1" s="3">
@@ -578,8 +577,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="40.7109375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
   <cols>
-    <col width="40.7109375" customWidth="1" style="1" min="1" max="5"/>
-    <col width="40.7109375" customWidth="1" style="1" min="6" max="16384"/>
+    <col width="40.7109375" customWidth="1" style="1" min="1" max="6"/>
+    <col width="40.7109375" customWidth="1" style="1" min="7" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customFormat="1" customHeight="1" s="2">
@@ -616,7 +615,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -624,10 +623,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="40.7109375" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
   <cols>
-    <col width="40.7109375" customWidth="1" style="6" min="1" max="6"/>
-    <col width="200.7109375" customWidth="1" style="6" min="7" max="7"/>
-    <col width="40.7109375" customWidth="1" style="6" min="8" max="11"/>
-    <col width="40.7109375" customWidth="1" style="6" min="12" max="16384"/>
+    <col width="40.7109375" customWidth="1" style="5" min="1" max="6"/>
+    <col width="200.7109375" customWidth="1" style="5" min="7" max="7"/>
+    <col width="40.7109375" customWidth="1" style="5" min="8" max="12"/>
+    <col width="40.7109375" customWidth="1" style="5" min="13" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customFormat="1" customHeight="1" s="4">
@@ -667,7 +666,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" s="5">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="inlineStr">
         <is>
           <t>1956801238</t>
@@ -678,18 +677,23 @@
           <t>1</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Создается</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2022-08-21 15:06:36.905554</t>
+          <t>2022-08-21 15:37:32.832707</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>мороженое, , чай, лимонад, смузи, смузи, мороженое, вафлю, молочный_коктель</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1" s="5">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" t="inlineStr">
         <is>
           <t>1956801238</t>
@@ -700,99 +704,41 @@
           <t>2</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Создается</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2022-08-21 15:06:44.242974</t>
+          <t>2022-08-21 15:38:51.982234</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-чай -чай -чай -смузи -мороженое -лимонад -вафлю -молочный_коктель -чай</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" s="5">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>1956801238</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Создается</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2022-08-21 15:16:08.011220</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1" s="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>1956801238</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Создается</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2022-08-21 15:17:43.980709</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1" s="5">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>1956801238</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Создается</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2022-08-21 15:18:01.481710</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1" s="5"/>
-    <row r="8" ht="15.75" customHeight="1" s="5"/>
-    <row r="9" ht="15.75" customHeight="1" s="5"/>
-    <row r="10" ht="15.75" customHeight="1" s="5"/>
-    <row r="11" ht="15.75" customHeight="1" s="5"/>
-    <row r="12" ht="15.75" customHeight="1" s="5"/>
-    <row r="13" ht="15.75" customHeight="1" s="5"/>
-    <row r="14" ht="15.75" customHeight="1" s="5"/>
-    <row r="15" ht="15.75" customHeight="1" s="5"/>
-    <row r="16" ht="15.75" customHeight="1" s="5"/>
-    <row r="17" ht="15.75" customHeight="1" s="5"/>
-    <row r="18" ht="15.75" customHeight="1" s="5"/>
-    <row r="19" ht="15.75" customHeight="1" s="5"/>
-    <row r="20" ht="15.75" customHeight="1" s="5"/>
-    <row r="21" ht="15.75" customHeight="1" s="5"/>
-    <row r="22" ht="15.75" customHeight="1" s="5"/>
+    <row r="4" ht="15.75" customHeight="1"/>
+    <row r="5" ht="15.75" customHeight="1"/>
+    <row r="6" ht="15.75" customHeight="1"/>
+    <row r="7" ht="15.75" customHeight="1"/>
+    <row r="8" ht="15.75" customHeight="1"/>
+    <row r="9" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -814,8 +760,8 @@
   <cols>
     <col width="40.7109375" customWidth="1" style="1" min="1" max="3"/>
     <col width="80.7109375" customWidth="1" style="1" min="4" max="4"/>
-    <col width="40.7109375" customWidth="1" style="1" min="5" max="9"/>
-    <col width="40.7109375" customWidth="1" style="1" min="10" max="16384"/>
+    <col width="40.7109375" customWidth="1" style="1" min="5" max="10"/>
+    <col width="40.7109375" customWidth="1" style="1" min="11" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customFormat="1" customHeight="1" s="2">

</xml_diff>